<commit_message>
fixed "disctrict" typo in PLZ population data
</commit_message>
<xml_diff>
--- a/main/python_package/geodata_berlin/data/other/districts/Statistik_Berlin_Brandenburg/manual_split/14_Einwohners_in_Berlin_am_31_Dezember_2023_nach_PLZ_Alter_gender.xlsx
+++ b/main/python_package/geodata_berlin/data/other/districts/Statistik_Berlin_Brandenburg/manual_split/14_Einwohners_in_Berlin_am_31_Dezember_2023_nach_PLZ_Alter_gender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente_D\Gits\geodata_berlin\main\python_package\geodata_berlin\data\other\districts\Statistik_Berlin_Brandenburg\manual_split\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33D9EFA-E93A-4113-8001-8B491FA109B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC68BA39-474F-460E-ACCE-D18A3B4D68AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -621,9 +621,6 @@
     <t>PLZ</t>
   </si>
   <si>
-    <t>disctrict</t>
-  </si>
-  <si>
     <t>total</t>
   </si>
   <si>
@@ -667,6 +664,9 @@
   </si>
   <si>
     <t>Marzahn-Hellersdorf</t>
+  </si>
+  <si>
+    <t>district</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1036,7 @@
   <dimension ref="A1:L238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,37 +1046,37 @@
         <v>197</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1236,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" s="4">
         <v>72</v>
@@ -1312,7 +1312,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8" s="4">
         <v>444</v>
@@ -1388,7 +1388,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="4">
         <v>33257</v>
@@ -1426,7 +1426,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C11" s="4">
         <v>37480</v>
@@ -1464,7 +1464,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" s="4">
         <v>40109</v>
@@ -1540,7 +1540,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" s="4">
         <v>29876</v>
@@ -2338,7 +2338,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C35" s="4">
         <v>15667</v>
@@ -2376,7 +2376,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C36" s="4">
         <v>14388</v>
@@ -2414,7 +2414,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C37" s="4">
         <v>15595</v>
@@ -2452,7 +2452,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C38" s="4">
         <v>6741</v>
@@ -2528,7 +2528,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C40" s="4">
         <v>11558</v>
@@ -2566,7 +2566,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C41" s="4">
         <v>13470</v>
@@ -2604,7 +2604,7 @@
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42" s="4">
         <v>13717</v>
@@ -2642,7 +2642,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C43" s="4">
         <v>13498</v>
@@ -2680,7 +2680,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C44" s="4">
         <v>10798</v>
@@ -2718,7 +2718,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C45" s="4">
         <v>11786</v>
@@ -2756,7 +2756,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C46" s="4">
         <v>13278</v>
@@ -2794,7 +2794,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C47" s="4">
         <v>17421</v>
@@ -2832,7 +2832,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C48" s="4">
         <v>17380</v>
@@ -2870,7 +2870,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C49" s="4">
         <v>10457</v>
@@ -2908,7 +2908,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C50" s="4">
         <v>3323</v>
@@ -2946,7 +2946,7 @@
         <v>44</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C51" s="4">
         <v>9876</v>
@@ -2984,7 +2984,7 @@
         <v>45</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C52" s="4">
         <v>2341</v>
@@ -3022,7 +3022,7 @@
         <v>45</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C53" s="4">
         <v>6816</v>
@@ -3060,7 +3060,7 @@
         <v>46</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C54" s="4">
         <v>13841</v>
@@ -3098,7 +3098,7 @@
         <v>47</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C55" s="4">
         <v>12182</v>
@@ -3136,7 +3136,7 @@
         <v>48</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C56" s="4">
         <v>1269</v>
@@ -3212,7 +3212,7 @@
         <v>48</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C58" s="4">
         <v>1493</v>
@@ -3250,7 +3250,7 @@
         <v>49</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C59" s="4">
         <v>95</v>
@@ -3326,7 +3326,7 @@
         <v>49</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C61" s="4">
         <v>3728</v>
@@ -3364,7 +3364,7 @@
         <v>50</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C62" s="4">
         <v>3092</v>
@@ -3402,7 +3402,7 @@
         <v>50</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C63" s="4">
         <v>2036</v>
@@ -3440,7 +3440,7 @@
         <v>51</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C64" s="4">
         <v>8976</v>
@@ -3478,7 +3478,7 @@
         <v>52</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C65" s="4">
         <v>452</v>
@@ -3516,7 +3516,7 @@
         <v>52</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C66" s="4">
         <v>10796</v>
@@ -3554,7 +3554,7 @@
         <v>53</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C67" s="4">
         <v>16208</v>
@@ -3592,7 +3592,7 @@
         <v>54</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C68" s="4">
         <v>16670</v>
@@ -3630,7 +3630,7 @@
         <v>55</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C69" s="4">
         <v>19525</v>
@@ -3668,7 +3668,7 @@
         <v>56</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C70" s="4">
         <v>15037</v>
@@ -3744,7 +3744,7 @@
         <v>57</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C72" s="4">
         <v>19078</v>
@@ -3820,7 +3820,7 @@
         <v>57</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C74" s="4">
         <v>3031</v>
@@ -3858,7 +3858,7 @@
         <v>59</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C75" s="4">
         <v>18567</v>
@@ -3934,7 +3934,7 @@
         <v>60</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C77" s="4">
         <v>28618</v>
@@ -3972,7 +3972,7 @@
         <v>61</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C78" s="4">
         <v>25270</v>
@@ -4010,7 +4010,7 @@
         <v>62</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C79" s="4">
         <v>24852</v>
@@ -4428,7 +4428,7 @@
         <v>72</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C90" s="4">
         <v>16452</v>
@@ -4466,7 +4466,7 @@
         <v>73</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C91" s="4">
         <v>17214</v>
@@ -4504,7 +4504,7 @@
         <v>74</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C92" s="4">
         <v>22095</v>
@@ -4542,7 +4542,7 @@
         <v>75</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C93" s="4">
         <v>25042</v>
@@ -4618,7 +4618,7 @@
         <v>76</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C95" s="4">
         <v>21373</v>
@@ -4656,7 +4656,7 @@
         <v>77</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C96" s="4">
         <v>16465</v>
@@ -4694,7 +4694,7 @@
         <v>78</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C97" s="4">
         <v>7902</v>
@@ -4732,7 +4732,7 @@
         <v>78</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C98" s="4">
         <v>12162</v>
@@ -4770,7 +4770,7 @@
         <v>79</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C99" s="4">
         <v>16161</v>
@@ -4808,7 +4808,7 @@
         <v>80</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C100" s="4">
         <v>1649</v>
@@ -4846,7 +4846,7 @@
         <v>80</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C101" s="4">
         <v>16444</v>
@@ -4884,7 +4884,7 @@
         <v>81</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C102" s="4">
         <v>19689</v>
@@ -4922,7 +4922,7 @@
         <v>81</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C103" s="4">
         <v>363</v>
@@ -4960,7 +4960,7 @@
         <v>82</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C104" s="4">
         <v>5222</v>
@@ -4998,7 +4998,7 @@
         <v>83</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C105" s="4">
         <v>20504</v>
@@ -5036,7 +5036,7 @@
         <v>84</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C106" s="4">
         <v>18011</v>
@@ -5074,7 +5074,7 @@
         <v>85</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C107" s="4">
         <v>21832</v>
@@ -5112,7 +5112,7 @@
         <v>86</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C108" s="4">
         <v>16102</v>
@@ -5150,7 +5150,7 @@
         <v>87</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C109" s="4">
         <v>24392</v>
@@ -5188,7 +5188,7 @@
         <v>88</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C110" s="4">
         <v>15793</v>
@@ -5226,7 +5226,7 @@
         <v>89</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C111" s="4">
         <v>21560</v>
@@ -5264,7 +5264,7 @@
         <v>90</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C112" s="4">
         <v>24704</v>
@@ -5302,7 +5302,7 @@
         <v>90</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C113" s="4">
         <v>719</v>
@@ -5340,7 +5340,7 @@
         <v>91</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C114" s="4">
         <v>45</v>
@@ -5378,7 +5378,7 @@
         <v>91</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C115" s="4">
         <v>14639</v>
@@ -5416,7 +5416,7 @@
         <v>92</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C116" s="4">
         <v>49</v>
@@ -5454,7 +5454,7 @@
         <v>92</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C117" s="4">
         <v>17622</v>
@@ -5530,7 +5530,7 @@
         <v>93</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C119" s="4">
         <v>21471</v>
@@ -5568,7 +5568,7 @@
         <v>94</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C120" s="4">
         <v>13073</v>
@@ -5606,7 +5606,7 @@
         <v>95</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C121" s="4">
         <v>17548</v>
@@ -5682,7 +5682,7 @@
         <v>96</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C123" s="4">
         <v>3</v>
@@ -6290,7 +6290,7 @@
         <v>113</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C139" s="4">
         <v>3</v>
@@ -6518,7 +6518,7 @@
         <v>118</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C145" s="4">
         <v>28899</v>
@@ -6556,7 +6556,7 @@
         <v>119</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C146" s="4">
         <v>17629</v>
@@ -6594,7 +6594,7 @@
         <v>120</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C147" s="4">
         <v>31367</v>
@@ -6670,7 +6670,7 @@
         <v>121</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C149" s="4">
         <v>45350</v>
@@ -6708,7 +6708,7 @@
         <v>122</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C150" s="4">
         <v>19912</v>
@@ -6746,7 +6746,7 @@
         <v>123</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C151" s="4">
         <v>29480</v>
@@ -6822,7 +6822,7 @@
         <v>124</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C153" s="4">
         <v>20083</v>
@@ -6860,7 +6860,7 @@
         <v>125</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C154" s="4">
         <v>31383</v>
@@ -6898,7 +6898,7 @@
         <v>126</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C155" s="4">
         <v>22060</v>
@@ -6936,7 +6936,7 @@
         <v>127</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C156" s="4">
         <v>20659</v>
@@ -6974,7 +6974,7 @@
         <v>128</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C157" s="4">
         <v>25123</v>
@@ -8874,7 +8874,7 @@
         <v>176</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C207" s="4">
         <v>3</v>
@@ -9026,7 +9026,7 @@
         <v>178</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C211" s="4">
         <v>19322</v>
@@ -9140,7 +9140,7 @@
         <v>179</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C214" s="4">
         <v>98</v>
@@ -9254,7 +9254,7 @@
         <v>180</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C217" s="4">
         <v>11378</v>
@@ -9292,7 +9292,7 @@
         <v>181</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C218" s="4">
         <v>12749</v>
@@ -9330,7 +9330,7 @@
         <v>182</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C219" s="4">
         <v>236</v>
@@ -9368,7 +9368,7 @@
         <v>183</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C220" s="4">
         <v>11521</v>
@@ -9406,7 +9406,7 @@
         <v>184</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C221" s="4">
         <v>14734</v>
@@ -9444,7 +9444,7 @@
         <v>185</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C222" s="4">
         <v>23701</v>
@@ -9520,7 +9520,7 @@
         <v>187</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C224" s="4">
         <v>11298</v>
@@ -9558,7 +9558,7 @@
         <v>188</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C225" s="4">
         <v>15470</v>
@@ -9596,7 +9596,7 @@
         <v>189</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C226" s="4">
         <v>17031</v>
@@ -9634,7 +9634,7 @@
         <v>190</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C227" s="4">
         <v>15517</v>
@@ -9672,7 +9672,7 @@
         <v>191</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C228" s="4">
         <v>18878</v>
@@ -9710,7 +9710,7 @@
         <v>192</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C229" s="4">
         <v>18581</v>
@@ -9748,7 +9748,7 @@
         <v>193</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C230" s="4">
         <v>18216</v>
@@ -9786,7 +9786,7 @@
         <v>193</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C231" s="4">
         <v>12</v>
@@ -9824,7 +9824,7 @@
         <v>194</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C232" s="4">
         <v>1265</v>
@@ -9862,7 +9862,7 @@
         <v>194</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C233" s="4">
         <v>15791</v>
@@ -9900,7 +9900,7 @@
         <v>195</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C234" s="4">
         <v>17229</v>
@@ -9938,7 +9938,7 @@
         <v>195</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C235" s="4">
         <v>386</v>
@@ -9976,7 +9976,7 @@
         <v>195</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C236" s="4">
         <v>1369</v>
@@ -10014,7 +10014,7 @@
         <v>196</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C237" s="4">
         <v>17572</v>
@@ -10052,7 +10052,7 @@
         <v>196</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C238" s="4">
         <v>28</v>

</xml_diff>